<commit_message>
informacion filtrad y grupos listos
</commit_message>
<xml_diff>
--- a/13 Artículos publicados.xlsx
+++ b/13 Artículos publicados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Artículos publicados</t>
   </si>
@@ -22,10 +22,31 @@
     <t>Nombre del Grupo</t>
   </si>
   <si>
-    <t>Ciencia y Tecnología de Biomoléculas de Interés Agroindustrial - CYTBIA</t>
-  </si>
-  <si>
-    <t>309.- Publicado en revista especializada: Uso de cartas de control para el análisis de calidad en manufactura de sacos de polipropileno  Colombia, Revista Biotecnología En El Sector Agropecuario Y Agroindustrial ISSN: 1909-9959, 2006 vol:4 fasc: 1 págs: 67 - 76, DOI:10.1142/30  Autores: SILVIO ANDRES MOSQUERA SANCHEZ, JENNY FLOR CABRERA, JHON JAIRO NARVAEZ</t>
+    <t>Posgrado en Aprovechamiento de Recursos Hidráulicos</t>
+  </si>
+  <si>
+    <t>ESTUDIO Y CONTROL DE LA CONTAMINACIÓN AMBIENTAL - ECCA</t>
+  </si>
+  <si>
+    <t>Bioprocesos y Flujos Reactivos</t>
+  </si>
+  <si>
+    <t>Limnología y Recursos Hídricos</t>
+  </si>
+  <si>
+    <t>273.- Publicado en revista especializada: Revisión de criterios y metodologías de diseño de redes para el monitoreo de la calidad de agua en ríos  Colombia, Avances En Recursos Hidráulicos ISSN: 0121-5701, 2008 vol:N/A fasc: 18 págs: 67 - 78, DOI:  Autores: A MORENO, FRANCISCO MAURICIO TORO BOTERO, LUIS FERNANDO CARVAJAL SERNA 
+ 274.- Publicado en revista especializada: Revisión de criterios y metodologías de diseño de redes para el monitoreo de la calidad de agua en ríos  Colombia, Avances En Recursos Hidráulicos ISSN: 0121-5701, 2008 vol:N/A fasc: 18 págs: 67 - 78, DOI:  Autores: LUIS FERNANDO CARVAJAL SERNA, A MORENO, MAURICIO TORO</t>
+  </si>
+  <si>
+    <t>103.- Publicado en revista especializada: Monitoreo y medición del ajuste del pH del agua tratada del río cauca mediante índices de estabilización  Colombia, Revista U.D.C.A Actualidad and Divulgacion Cientifica ISSN: 0123-4226, 2014 vol:17 fasc: 2 págs: 563 - 575, DOI:  Autores: PATRICIA TORRES LOZADA, KAREN ALEJANDRA BUENO ZABALA, LUIS GERMAN DELGADO 
+ 176.- Publicado en revista especializada: Propuesta metodológica para localización de estaciones de monitoreo de calidad de agua en redes de distribución utilizando sistemas de información geográfica  Colombia, Revista Facultad de Ingenieria ISSN: 0120-6230, 2009 vol:49 fasc: N/A págs: 129 - 140, DOI:  Autores: CAMILO HERNAN CRUZ VELEZ, CAROLINA MONTOYA PACHONGO, DIANA LOAIZA, PATRICIA TORRES LOZADA, JUAN CARLOS ESCOBAR RIVERA, LUIS GERMAN DELGADO</t>
+  </si>
+  <si>
+    <t>49.- Publicado en revista especializada: Monitoreo y medición del ajuste del pH del agua tratada del río Cauca mediante índices de estabilización  Colombia, Revista U.D.C.A Actualidad and Divulgacion Cientifica ISSN: 0123-4226, 2014 vol:17 fasc: 2 págs: 563 - 575, DOI:  Autores: KAREN ALEJANDRA BUENO ZABALA, PATRICIA TORRES LOZADA, LUIS GERMAN DELGADO CABRERA</t>
+  </si>
+  <si>
+    <t>38.- Corto (Resumen): Monitoreo de la asociacion de especies icticas, aguas arriba del embalse Amani, rio La Miel aguas abajode la presa de la central hidroelectrica Miel I- y afluentes principales (Rios Manso y Samana) duante 2008, Colombia  Colombia, Actualidades Biológicas ISSN: 0304-3584, 2009 vol:31 fasc: N/A págs: 54 - 54, DOI:  Autores: MARIA ISABEL RIOS PULGARIN, ALEXANDRA ARANGO ROJAS, ESTEBAN PELAEZ SANCHEZ 
+ 44.- Publicado en revista especializada: Monitoreo de la asociaciones de especies ícticas, aguas arriba del embalse Amaní, Río La Miel aguas abajo de la presa de la Hidroeléctrica Miel I y afluentes principales (Ríos Manso y Samaná) durante 2008  Colombia, Actualidades Biológicas ISSN: 0304-3584, 2009 vol:31 fasc: N/A págs: 54 - 54, DOI:  Autores: MARIA ISABEL RIOS PULGARIN, GLORIA ALEXANDRA ARANGO ROJAS, ESTEBAN PELAEZ SANCHEZ</t>
   </si>
 </sst>
 </file>
@@ -383,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +423,31 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>